<commit_message>
fixing more variation iterations
</commit_message>
<xml_diff>
--- a/datasheets/allele.xlsx
+++ b/datasheets/allele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oriol/Desktop/beacon-ri-tools-v2/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCE79BB-C3A1-FC4D-859C-F42086565BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769AD7C2-E7F1-5B41-8032-C5FEE3647BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analyses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="479">
   <si>
     <t>aligner</t>
   </si>
@@ -928,6 +928,42 @@
     <t>variation|referenceBases</t>
   </si>
   <si>
+    <t>variation|state|components|location|_id</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|chr</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|interval</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|interval|end</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|interval|start</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|interval|type</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|sequence_id</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|species_id</t>
+  </si>
+  <si>
+    <t>variation|state|components|location|type</t>
+  </si>
+  <si>
+    <t>variation|state|components|reverse_complement</t>
+  </si>
+  <si>
+    <t>variation|state|components|sequence</t>
+  </si>
+  <si>
+    <t>variation|state|components|type</t>
+  </si>
+  <si>
     <t>variation|state|count|comparator</t>
   </si>
   <si>
@@ -955,9 +991,39 @@
     <t>variation|state|location|interval|end</t>
   </si>
   <si>
+    <t>variation|state|location|interval|end|comparator</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|end|max</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|end|min</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|end|type</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|end|value</t>
+  </si>
+  <si>
     <t>variation|state|location|interval|start</t>
   </si>
   <si>
+    <t>variation|state|location|interval|start|comparator</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|start|max</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|start|min</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|start|type</t>
+  </si>
+  <si>
+    <t>variation|state|location|interval|start|value</t>
+  </si>
+  <si>
     <t>variation|state|location|interval|type</t>
   </si>
   <si>
@@ -979,6 +1045,15 @@
     <t>variation|state|seq_expr|location|interval</t>
   </si>
   <si>
+    <t>variation|state|seq_expr|location|interval|end</t>
+  </si>
+  <si>
+    <t>variation|state|seq_expr|location|interval|start</t>
+  </si>
+  <si>
+    <t>variation|state|seq_expr|location|interval|type</t>
+  </si>
+  <si>
     <t>variation|state|seq_expr|location|sequence_id</t>
   </si>
   <si>
@@ -1009,6 +1084,33 @@
     <t>variation|variantType</t>
   </si>
   <si>
+    <t>SO:0001777</t>
+  </si>
+  <si>
+    <t>somatic variant</t>
+  </si>
+  <si>
+    <t>bs001104</t>
+  </si>
+  <si>
+    <t>var00001</t>
+  </si>
+  <si>
+    <t>q22.4</t>
+  </si>
+  <si>
+    <t>q22.3</t>
+  </si>
+  <si>
+    <t>CytobandInterval</t>
+  </si>
+  <si>
+    <t>taxonomy:9606</t>
+  </si>
+  <si>
+    <t>ChromosomeLocation</t>
+  </si>
+  <si>
     <t>diseases|ageOfOnset</t>
   </si>
   <si>
@@ -1345,382 +1447,34 @@
     <t>runDate</t>
   </si>
   <si>
-    <t>bwa-0.5.9</t>
-  </si>
-  <si>
-    <t>2015-09-30</t>
-  </si>
-  <si>
-    <t>HG00096</t>
-  </si>
-  <si>
-    <t>UK1_analysisId_1</t>
-  </si>
-  <si>
-    <t>1000G-low-coverage-WGS</t>
-  </si>
-  <si>
-    <t>https://www.nature.com/articles/nature15393</t>
-  </si>
-  <si>
-    <t>SRR00000001</t>
-  </si>
-  <si>
-    <t>GATK4.0</t>
-  </si>
-  <si>
-    <t>HG00097</t>
-  </si>
-  <si>
-    <t>UK1_analysisId_2</t>
-  </si>
-  <si>
-    <t>SRR00000002</t>
-  </si>
-  <si>
-    <t>HG00099</t>
-  </si>
-  <si>
-    <t>UK1_analysisId_3</t>
-  </si>
-  <si>
-    <t>SRR00000003</t>
-  </si>
-  <si>
-    <t>HG00100</t>
-  </si>
-  <si>
-    <t>UK1_analysisId_4</t>
-  </si>
-  <si>
-    <t>SRR00000004</t>
-  </si>
-  <si>
-    <t>HG00101</t>
-  </si>
-  <si>
-    <t>UK1_analysisId_5</t>
-  </si>
-  <si>
-    <t>SRR00000005</t>
-  </si>
-  <si>
-    <t>EFO:0009654</t>
-  </si>
-  <si>
-    <t>reference sample</t>
-  </si>
-  <si>
-    <t>2020-09-11</t>
-  </si>
-  <si>
-    <t>P40Y1M1D</t>
-  </si>
-  <si>
-    <t>{"BioSamples": {"accession": "SAMEA7082831","externalUrl": "https://www.ebi.ac.uk/biosamples/SAMEA7082831"},"EGAsampleId": "EGAN00002589008","characteristics": [{"organism": [{"ontologyTerms": ["http://purl.obolibrary.org/obo/NCBITaxon_9606"],"text": "Homo sapiens"}]}],"sampleName": "synthetic_sample_3","taxId": 9606}</t>
-  </si>
-  <si>
-    <t>UBERON:0000178</t>
-  </si>
-  <si>
-    <t>blood</t>
-  </si>
-  <si>
-    <t>study-defined</t>
-  </si>
-  <si>
-    <t>{"diseases": {"acute bronchitis": 121,"agranulocytosis": 111,"asthma": 134,"bipolar affective disorder": 134,"cardiomyopathy": 133,"dental caries": 139,"eating disorders": 134,"fibrosis and cirrhosis of liver": 132,"gastro-oesophageal reflux disease": 140,"haemorrhoids": 127,"influenza due to certain identified influenza virus": 135,"insulin-dependent diabetes mellitus": 165,"iron deficiency anaemia": 142,"multiple sclerosis": 125,"obesity": 136,"sarcoidosis": 136,"schizophrenia": 138,"thyroiditis": 141,"varicose veins of lower extremities": 139}}</t>
-  </si>
-  <si>
-    <t>{"ethnicities": {"African": 119,"Any other Asian background": 120,"Any other Black background": 104,"Any other mixed background": 92,"Any other white background": 114,"Asian or Asian British": 125,"Bangladeshi": 96,"Black or Black British": 131,"British": 114,"Caribbean": 127,"Chinese": 100,"Indian": 110,"Irish": 111,"Mixed": 127,"Other ethnic group": 116,"Pakistani": 115,"White": 105,"White and Asian": 114,"White and Black African": 115,"White and Black Caribbean": 132}}</t>
-  </si>
-  <si>
-    <t>{"genders": {"female": 1271,"male": 1233}}</t>
-  </si>
-  <si>
-    <t>CINECA_synthetic_cohort_UK1</t>
-  </si>
-  <si>
-    <t>P65Y</t>
-  </si>
-  <si>
-    <t>P18Y</t>
-  </si>
-  <si>
-    <t>NCIT:C16576,NCIT:C20197</t>
-  </si>
-  <si>
-    <t>female,male</t>
-  </si>
-  <si>
-    <t>GAZ:00150372</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>CINECA synthetic cohort UK1</t>
-  </si>
-  <si>
-    <t>2021-12-29T20:33:40Z</t>
-  </si>
-  <si>
-    <t>DUO:0000019,DUO:00000020</t>
-  </si>
-  <si>
-    <t>publication required,publication required</t>
-  </si>
-  <si>
-    <t>7-1-19,7-1-19</t>
-  </si>
-  <si>
-    <t>Please note: This synthetic data set (with cohort participants / subjects marked with FAKE) has no identifiable data and cannot be used to make any inference about cohort data or results. The purpose of this dataset is to aid development of technical implementations for cohort data discovery, harmonization, access, and federated analysis. In support of FAIRness in data sharing, this dataset is made freely available under the Creative Commons Licence (CC-BY). Please ensure this preamble is included with this dataset and that the CINECA project (funding: EC H2020 grant 825775) is acknowledged. For any questions please contact isuru@ebi.ac.uk or cthomas@ebi.ac.uk This dataset (CINECA_synthetic_cohort_EUROPE_UK1) consists of 2521 samples which have genetic data based on 1000 Genomes data (https://www.nature.com/articles/nature15393), and synthetic subject attributes and phenotypic data derived from UKBiobank (https://journals.plos.org/plosmedicine/article?id=10.1371/journal.pmed.1001779). These data were initially derived using the TOFU tool (https://github.com/spiros/tofu), which generates randomly generated values based on the UKBiobank data dictionary. Categorical values were randomly generated based on the data dictionary, continuous variables generated based on the distribution of values reported by the UK Biobank showcase, and date / time values were random. Additionally we split the phenotypes and attributes into 4 main classes - general, cancer, diabetes mellitus, and cardiac. We assigned the general attributes to all the samples, and the cardiac / diabetes mellitus / cancer attributes to a proportion of the total samples. Once the initial set of phenotypes and attributes were generated, the data data was checked for consistency and where possible dependent attributes were calculated from the independent variables generated by TOFU. For example, BMI was calculated from height and weight data, and age at death generated by date of death and date of birth. These data were then loaded to the development instance of Biosamples (https://www.ebi.ac.uk/biosamples/) which accessioned each of the samples. The genetic data are derived from the 1000 Genomes Phase 3 release (https://www.internationalgenome.org/category/phase-3/). The genotype data consists of a single joint call vcf files with call genotypes for all 2504 samples, plus bed, bim, fam, and nosex files generated via plink for these samples and genotypes. The genotype data has had a variety of errors introduced to mimic real data and as a test for quality control pipelines. These include gender mismatches, ethnic background mislabelling and low call rates for a randomly chosen subset of sample data as well as deviations from Hardy Weinberg equilibrium and low call rates for a random selection of variants. Additionally 40 samples have raw genetic data available in the form of both bam and cram files, including unmapped data. The gender of the samples in the 1000 genomes data has been matched to the synthetic phenotypic data generated for these samples. The genetic data was then linked to the synthetic data in BioSamples, and submitted to EGA.","externalUrl": "https://ega-archive.org/datasets/EGAD00001006673/</t>
-  </si>
-  <si>
-    <t>https://ega-archive.org/datasets/EGAD00001006673/</t>
-  </si>
-  <si>
-    <t>CINECA_synthetic_cohort_EUROPE_UK1</t>
-  </si>
-  <si>
-    <t>{"beacon": {"contact": "manuel.rueda@crg.eu","mapping": "Manuel Rueda","version": "v2.0"},"dataset": {"derived": [{"EGA": {"contact": "helpdesk@ega-archive.org","externalUrl": "https://ega-archive.org/datasets/EGAD00001006673","license": {"$ref": "#/dataUseConditions/duoDataUse"}}},{"BioSamples": {"contact": "biosamples@ebi.ac.uk","externalUrl": "https://www.ebi.ac.uk/biosamples","license": "Creative Commons Licence (CC-BY)"}}],"origin": [{"CINECAprojectEU": {"contact": "cthomas@ebi.ac.uk","externalUrl": "https://www.cineca-project.eu/cineca-synthetic-dataset","license": "Creative Commons Licence (CC-BY)","managers": " Coline Thomas, Isuru Liyanage and Dylan Spalding"}},{"1000Genomes": {"externalUrl": "https://www.internationalgenome.org/category/phase-3","license": "CC BY-NC-SA 3.0","version": "v5a phase 3 VCF"}}]}}</t>
-  </si>
-  <si>
-    <t>v1.0</t>
-  </si>
-  <si>
-    <t>NCIT:C42331</t>
-  </si>
-  <si>
-    <t>African</t>
-  </si>
-  <si>
-    <t>fake1</t>
-  </si>
-  <si>
-    <t>OPCS4:L46.3</t>
-  </si>
-  <si>
-    <t>OPCS(v4-0.0):Ligation of visceral branch of abdominal aorta NEC</t>
-  </si>
-  <si>
-    <t>LOINC:35925-4|LOINC:3141-9|LOINC:8308-9</t>
-  </si>
-  <si>
-    <t>BMI|Weight|Height-standing</t>
-  </si>
-  <si>
-    <t>2021-09-24|2021-09-24|2021-09-24</t>
-  </si>
-  <si>
-    <t>NCIT:C49671|NCIT:C28252|NCIT:C49668</t>
-  </si>
-  <si>
-    <t>Kilogram per Square Meter|Kilogram|Centimeter</t>
-  </si>
-  <si>
-    <t>26.63838307|85.6358|179.2973</t>
-  </si>
-  <si>
-    <t>NCIT:C20197</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>NCIT:C41261</t>
-  </si>
-  <si>
-    <t>British</t>
-  </si>
-  <si>
-    <t>GAZ:00002641</t>
-  </si>
-  <si>
-    <t>England</t>
-  </si>
-  <si>
-    <t>fake2</t>
-  </si>
-  <si>
-    <t>OPCS4:K06.1</t>
-  </si>
-  <si>
-    <t>OPCS(v4-0.0):Repositioning of transposed great arteries</t>
-  </si>
-  <si>
-    <t>25.62278441|64.5722|158.7485</t>
-  </si>
-  <si>
-    <t>NCIT:C16576</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>NCIT:C41260</t>
-  </si>
-  <si>
-    <t>Asian or Asian British</t>
-  </si>
-  <si>
-    <t>GAZ:00002640</t>
-  </si>
-  <si>
-    <t>Wales</t>
-  </si>
-  <si>
-    <t>fake3</t>
-  </si>
-  <si>
-    <t>OPCS4:T89.4</t>
-  </si>
-  <si>
-    <t>OPCS(v4-0.0):Cannulation of lymphatic duct</t>
-  </si>
-  <si>
-    <t>22.35976255|64.4364|169.7587</t>
-  </si>
-  <si>
-    <t>NCIT:C67109</t>
-  </si>
-  <si>
-    <t>White and Asian</t>
-  </si>
-  <si>
-    <t>fake4</t>
-  </si>
-  <si>
-    <t>OPCS4:T77.2</t>
-  </si>
-  <si>
-    <t>OPCS(v4-0.0):Wide excision of muscle</t>
-  </si>
-  <si>
-    <t>28.27885509|74.4885|162.2982</t>
-  </si>
-  <si>
-    <t>White and Black African</t>
-  </si>
-  <si>
-    <t>fake5</t>
-  </si>
-  <si>
-    <t>OPCS4:Z01.4</t>
-  </si>
-  <si>
-    <t>OPCS(v4-0.0):Tissue of occipital lobe of brain</t>
-  </si>
-  <si>
-    <t>25.52066954|82.3472|179.6298</t>
-  </si>
-  <si>
-    <t>PAIRED</t>
-  </si>
-  <si>
-    <t>RANDOM</t>
-  </si>
-  <si>
-    <t>GENEPIO:0001966</t>
-  </si>
-  <si>
-    <t>genomic Source</t>
-  </si>
-  <si>
-    <t>Short read Illumina WGS sequencing</t>
-  </si>
-  <si>
-    <t>Illumina</t>
-  </si>
-  <si>
-    <t>OBI:0002048</t>
-  </si>
-  <si>
-    <t>Illumina HiSeq 2000</t>
-  </si>
-  <si>
-    <t>Allele</t>
-  </si>
-  <si>
-    <t>ChromosomeLocation</t>
-  </si>
-  <si>
-    <t>taxonomy:9606</t>
-  </si>
-  <si>
-    <t>CytobandInterval</t>
-  </si>
-  <si>
-    <t>q22.3</t>
-  </si>
-  <si>
-    <t>q22.4</t>
-  </si>
-  <si>
-    <t>LiteralSequenceExpression</t>
-  </si>
-  <si>
-    <t>22chr</t>
-  </si>
-  <si>
-    <t>SO:0001777</t>
-  </si>
-  <si>
-    <t>somatic variant</t>
-  </si>
-  <si>
-    <t>bs001104</t>
-  </si>
-  <si>
-    <t>var00001</t>
+    <t>taxonomy:6609</t>
+  </si>
+  <si>
+    <t>SequenceInterval</t>
+  </si>
+  <si>
+    <t>VRS:0101</t>
+  </si>
+  <si>
+    <t>SequenceLocation</t>
+  </si>
+  <si>
+    <t>DerivedSequenceExpression</t>
+  </si>
+  <si>
+    <t>DefiniteRange</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FFB6B6B6"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF12B300"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF66CCFF"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1747,24 +1501,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2077,194 +1822,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:L6"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:B8"/>
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="9" max="12" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="10.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="E2" t="s">
-        <v>441</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C3" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="E3" t="s">
-        <v>447</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C4" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="E4" t="s">
-        <v>450</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C5" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="E5" t="s">
-        <v>453</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="E6" t="s">
-        <v>456</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -2274,441 +1874,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C1:CR6"/>
+  <dimension ref="A1:CP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:96" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="S1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="T1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="U1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="V1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="W1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Z1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AA1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AB1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AC1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AD1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AE1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AF1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AG1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AH1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AI1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AJ1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AK1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AL1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AM1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AN1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AO1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AP1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AQ1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AR1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AS1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AT1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AU1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AV1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AW1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AX1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AY1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AZ1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="BA1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="BB1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="BC1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="BD1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="BE1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="BF1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="BG1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="BH1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="BI1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BJ1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="BK1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="BL1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="BM1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="BN1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="BO1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="BP1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="BQ1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="BR1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="BS1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="BT1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="BU1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="BV1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="BW1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="BX1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="BY1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="BZ1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="CA1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="CB1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CC1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="CD1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="CE1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="CF1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="CG1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="CH1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="CI1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="CJ1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="CK1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="CL1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="CM1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="CN1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="CO1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="CP1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CR1" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="3:96" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="K2" t="s">
-        <v>441</v>
-      </c>
-      <c r="L2" t="s">
-        <v>441</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>464</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="3" spans="3:96" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="K3" t="s">
-        <v>447</v>
-      </c>
-      <c r="L3" t="s">
-        <v>447</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>464</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="4" spans="3:96" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="K4" t="s">
-        <v>450</v>
-      </c>
-      <c r="L4" t="s">
-        <v>450</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>464</v>
-      </c>
-      <c r="CJ4" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="5" spans="3:96" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="K5" t="s">
-        <v>453</v>
-      </c>
-      <c r="L5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="CI5" t="s">
-        <v>464</v>
-      </c>
-      <c r="CJ5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="6" spans="3:96" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="K6" t="s">
-        <v>456</v>
-      </c>
-      <c r="L6" t="s">
-        <v>456</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="CI6" t="s">
-        <v>464</v>
-      </c>
-      <c r="CJ6" t="s">
-        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -2718,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="C1:CR2"/>
+  <dimension ref="C1:CR1"/>
   <sheetViews>
     <sheetView topLeftCell="CA1" workbookViewId="0">
-      <selection activeCell="CR1" sqref="CR1"/>
+      <selection activeCell="CA2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3008,67 +2463,6 @@
       </c>
       <c r="CR1" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="3:96" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" s="4">
-        <v>1705</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="R2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" s="4">
-        <v>2287</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="U2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V2" s="4">
-        <v>1597</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="BN2" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="BO2" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="BT2" s="3"/>
-      <c r="BU2" s="3"/>
-      <c r="BV2" s="3"/>
-      <c r="BW2" s="3"/>
-      <c r="BY2" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="BZ2" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="CA2" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="CB2" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="CR2" s="3" t="s">
-        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -3078,519 +2472,570 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="C1:O2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" t="s">
+        <v>195</v>
+      </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s">
-        <v>200</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>201</v>
+        <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>202</v>
       </c>
       <c r="M1" t="s">
-        <v>193</v>
-      </c>
-      <c r="N1" t="s">
-        <v>202</v>
-      </c>
-      <c r="O1" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>486</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="https://ega-archive.org/datasets/EGAD00001006673/" xr:uid="{9CF3A258-CA26-484C-A5F6-0F412DE59F96}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{B61B76EE-E2B5-AA41-9E22-BD994CC2F386}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="C1:DU2"/>
+  <dimension ref="A1:ER2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="BA2" sqref="BA2"/>
+    <sheetView tabSelected="1" topLeftCell="DT1" workbookViewId="0">
+      <selection activeCell="DV1" sqref="DV1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:125" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:148" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
       <c r="C1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="I1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="L1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="M1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="N1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="O1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="P1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="Q1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="R1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="S1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="T1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="U1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="V1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="W1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="X1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="Y1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="Z1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AA1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AB1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AC1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AD1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AE1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="AF1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AG1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AH1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AI1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AJ1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AK1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AL1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AM1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AN1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AO1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="AP1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="AQ1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AR1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AS1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AT1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AU1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AV1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AW1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AX1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AY1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AZ1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="BA1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="BB1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="BC1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="BD1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="BE1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="BF1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BG1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BH1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="BJ1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="BK1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="BL1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="BM1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="BN1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="BO1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="BP1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="BQ1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="BR1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="BS1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="BT1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="BU1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="BV1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="BW1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="BX1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="BY1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="BZ1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="CA1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="CB1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="CC1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="CD1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="CE1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="CF1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="CG1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="CH1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="CI1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="CJ1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="CK1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="CL1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="CM1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="CN1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="CO1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="CP1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="CQ1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="CR1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="CS1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="CT1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="CU1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="CV1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="CW1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="CX1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="CY1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="CZ1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="DA1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="DB1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="DC1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="DD1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="DE1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="DF1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="DG1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="DH1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="DI1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="DJ1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="DK1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="DL1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="DM1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="DN1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="DO1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="DP1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="DQ1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="DR1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="DS1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="DT1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="DU1" t="s">
-        <v>326</v>
+        <v>328</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>329</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>330</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>331</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>332</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>333</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>334</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>335</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>336</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>337</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>338</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>339</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>340</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>341</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>342</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>343</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>344</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>345</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>346</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>347</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>348</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>349</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>350</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>351</v>
       </c>
     </row>
-    <row r="2" spans="3:125" x14ac:dyDescent="0.2">
-      <c r="C2" s="9" t="s">
-        <v>545</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>547</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="CB2">
+    <row r="2" spans="1:148" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ2">
         <v>22</v>
       </c>
-      <c r="CD2" t="s">
-        <v>542</v>
-      </c>
-      <c r="CJ2" s="9" t="s">
-        <v>541</v>
+      <c r="CB2" t="s">
+        <v>356</v>
+      </c>
+      <c r="CH2" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>358</v>
       </c>
       <c r="CP2" t="s">
-        <v>540</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>539</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>538</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>544</v>
-      </c>
-      <c r="DS2" s="9" t="s">
-        <v>543</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>537</v>
+        <v>359</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>360</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>473</v>
+      </c>
+      <c r="DU2">
+        <v>1</v>
+      </c>
+      <c r="DV2">
+        <v>0</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>478</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>474</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>475</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>476</v>
+      </c>
+      <c r="EP2" s="2" t="s">
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -3600,660 +3045,428 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="C1:EJ6"/>
+  <dimension ref="A1:EH1"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="CU2" sqref="CU2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:140" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:138" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
+        <v>362</v>
+      </c>
       <c r="C1" t="s">
-        <v>327</v>
+        <v>363</v>
       </c>
       <c r="D1" t="s">
-        <v>328</v>
+        <v>364</v>
       </c>
       <c r="E1" t="s">
-        <v>329</v>
+        <v>365</v>
       </c>
       <c r="F1" t="s">
-        <v>330</v>
+        <v>366</v>
       </c>
       <c r="G1" t="s">
-        <v>331</v>
+        <v>367</v>
       </c>
       <c r="H1" t="s">
-        <v>332</v>
+        <v>368</v>
       </c>
       <c r="I1" t="s">
-        <v>333</v>
+        <v>369</v>
       </c>
       <c r="J1" t="s">
-        <v>334</v>
+        <v>370</v>
       </c>
       <c r="K1" t="s">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="L1" t="s">
-        <v>336</v>
+        <v>372</v>
       </c>
       <c r="M1" t="s">
-        <v>337</v>
+        <v>373</v>
       </c>
       <c r="N1" t="s">
-        <v>338</v>
+        <v>374</v>
       </c>
       <c r="O1" t="s">
-        <v>339</v>
+        <v>375</v>
       </c>
       <c r="P1" t="s">
-        <v>340</v>
+        <v>376</v>
       </c>
       <c r="Q1" t="s">
-        <v>341</v>
+        <v>377</v>
       </c>
       <c r="R1" t="s">
-        <v>342</v>
+        <v>378</v>
       </c>
       <c r="S1" t="s">
-        <v>343</v>
+        <v>379</v>
       </c>
       <c r="T1" t="s">
-        <v>344</v>
+        <v>380</v>
       </c>
       <c r="U1" t="s">
-        <v>345</v>
+        <v>381</v>
       </c>
       <c r="V1" t="s">
-        <v>346</v>
+        <v>382</v>
       </c>
       <c r="W1" t="s">
-        <v>347</v>
+        <v>383</v>
       </c>
       <c r="X1" t="s">
-        <v>348</v>
+        <v>384</v>
       </c>
       <c r="Y1" t="s">
-        <v>349</v>
+        <v>385</v>
       </c>
       <c r="Z1" t="s">
-        <v>350</v>
+        <v>386</v>
       </c>
       <c r="AA1" t="s">
-        <v>351</v>
+        <v>387</v>
       </c>
       <c r="AB1" t="s">
-        <v>352</v>
+        <v>388</v>
       </c>
       <c r="AC1" t="s">
-        <v>353</v>
+        <v>389</v>
       </c>
       <c r="AD1" t="s">
-        <v>354</v>
+        <v>3</v>
       </c>
       <c r="AE1" t="s">
-        <v>355</v>
+        <v>5</v>
       </c>
       <c r="AF1" t="s">
-        <v>3</v>
+        <v>390</v>
       </c>
       <c r="AG1" t="s">
-        <v>5</v>
+        <v>391</v>
       </c>
       <c r="AH1" t="s">
-        <v>356</v>
+        <v>392</v>
       </c>
       <c r="AI1" t="s">
-        <v>357</v>
+        <v>393</v>
       </c>
       <c r="AJ1" t="s">
-        <v>358</v>
+        <v>394</v>
       </c>
       <c r="AK1" t="s">
-        <v>359</v>
+        <v>395</v>
       </c>
       <c r="AL1" t="s">
-        <v>360</v>
+        <v>396</v>
       </c>
       <c r="AM1" t="s">
-        <v>361</v>
+        <v>397</v>
       </c>
       <c r="AN1" t="s">
-        <v>362</v>
+        <v>398</v>
       </c>
       <c r="AO1" t="s">
-        <v>363</v>
+        <v>399</v>
       </c>
       <c r="AP1" t="s">
-        <v>364</v>
+        <v>400</v>
       </c>
       <c r="AQ1" t="s">
-        <v>365</v>
+        <v>401</v>
       </c>
       <c r="AR1" t="s">
-        <v>366</v>
+        <v>402</v>
       </c>
       <c r="AS1" t="s">
-        <v>367</v>
+        <v>403</v>
       </c>
       <c r="AT1" t="s">
-        <v>368</v>
+        <v>404</v>
       </c>
       <c r="AU1" t="s">
-        <v>369</v>
+        <v>405</v>
       </c>
       <c r="AV1" t="s">
-        <v>370</v>
+        <v>406</v>
       </c>
       <c r="AW1" t="s">
-        <v>371</v>
+        <v>407</v>
       </c>
       <c r="AX1" t="s">
-        <v>372</v>
+        <v>408</v>
       </c>
       <c r="AY1" t="s">
-        <v>373</v>
+        <v>409</v>
       </c>
       <c r="AZ1" t="s">
-        <v>374</v>
+        <v>410</v>
       </c>
       <c r="BA1" t="s">
-        <v>375</v>
+        <v>411</v>
       </c>
       <c r="BB1" t="s">
-        <v>376</v>
+        <v>412</v>
       </c>
       <c r="BC1" t="s">
-        <v>377</v>
+        <v>413</v>
       </c>
       <c r="BD1" t="s">
-        <v>378</v>
+        <v>414</v>
       </c>
       <c r="BE1" t="s">
-        <v>379</v>
+        <v>415</v>
       </c>
       <c r="BF1" t="s">
-        <v>380</v>
+        <v>416</v>
       </c>
       <c r="BG1" t="s">
-        <v>381</v>
+        <v>417</v>
       </c>
       <c r="BH1" t="s">
-        <v>382</v>
+        <v>418</v>
       </c>
       <c r="BI1" t="s">
-        <v>383</v>
+        <v>419</v>
       </c>
       <c r="BJ1" t="s">
-        <v>384</v>
+        <v>420</v>
       </c>
       <c r="BK1" t="s">
-        <v>385</v>
+        <v>421</v>
       </c>
       <c r="BL1" t="s">
-        <v>386</v>
+        <v>422</v>
       </c>
       <c r="BM1" t="s">
-        <v>387</v>
+        <v>423</v>
       </c>
       <c r="BN1" t="s">
-        <v>388</v>
+        <v>424</v>
       </c>
       <c r="BO1" t="s">
-        <v>389</v>
+        <v>425</v>
       </c>
       <c r="BP1" t="s">
-        <v>390</v>
+        <v>426</v>
       </c>
       <c r="BQ1" t="s">
-        <v>391</v>
+        <v>427</v>
       </c>
       <c r="BR1" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="BS1" t="s">
-        <v>393</v>
+        <v>429</v>
       </c>
       <c r="BT1" t="s">
-        <v>394</v>
+        <v>430</v>
       </c>
       <c r="BU1" t="s">
-        <v>395</v>
+        <v>431</v>
       </c>
       <c r="BV1" t="s">
-        <v>396</v>
+        <v>432</v>
       </c>
       <c r="BW1" t="s">
-        <v>397</v>
+        <v>433</v>
       </c>
       <c r="BX1" t="s">
-        <v>398</v>
+        <v>434</v>
       </c>
       <c r="BY1" t="s">
-        <v>399</v>
+        <v>435</v>
       </c>
       <c r="BZ1" t="s">
-        <v>400</v>
+        <v>436</v>
       </c>
       <c r="CA1" t="s">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="CB1" t="s">
-        <v>402</v>
+        <v>438</v>
       </c>
       <c r="CC1" t="s">
-        <v>403</v>
+        <v>439</v>
       </c>
       <c r="CD1" t="s">
-        <v>404</v>
+        <v>440</v>
       </c>
       <c r="CE1" t="s">
-        <v>405</v>
+        <v>441</v>
       </c>
       <c r="CF1" t="s">
-        <v>406</v>
+        <v>442</v>
       </c>
       <c r="CG1" t="s">
-        <v>407</v>
+        <v>443</v>
       </c>
       <c r="CH1" t="s">
-        <v>408</v>
+        <v>444</v>
       </c>
       <c r="CI1" t="s">
-        <v>409</v>
+        <v>445</v>
       </c>
       <c r="CJ1" t="s">
-        <v>410</v>
+        <v>446</v>
       </c>
       <c r="CK1" t="s">
-        <v>411</v>
+        <v>447</v>
       </c>
       <c r="CL1" t="s">
-        <v>412</v>
+        <v>448</v>
       </c>
       <c r="CM1" t="s">
-        <v>413</v>
+        <v>449</v>
       </c>
       <c r="CN1" t="s">
-        <v>414</v>
+        <v>450</v>
       </c>
       <c r="CO1" t="s">
-        <v>415</v>
+        <v>451</v>
       </c>
       <c r="CP1" t="s">
-        <v>416</v>
+        <v>452</v>
       </c>
       <c r="CQ1" t="s">
-        <v>417</v>
+        <v>56</v>
       </c>
       <c r="CR1" t="s">
-        <v>418</v>
+        <v>57</v>
       </c>
       <c r="CS1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="CT1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="CU1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="CV1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="CW1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="CX1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="CY1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="CZ1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="DA1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="DB1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="DC1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="DD1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="DE1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="DF1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="DG1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="DH1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="DI1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="DJ1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="DK1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="DL1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="DM1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="DN1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="DO1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="DP1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="DQ1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="DR1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="DS1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="DT1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="DU1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="DV1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="DW1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="DX1" t="s">
-        <v>87</v>
+        <v>453</v>
       </c>
       <c r="DY1" t="s">
-        <v>88</v>
+        <v>454</v>
       </c>
       <c r="DZ1" t="s">
-        <v>419</v>
+        <v>455</v>
       </c>
       <c r="EA1" t="s">
-        <v>420</v>
+        <v>456</v>
       </c>
       <c r="EB1" t="s">
-        <v>421</v>
+        <v>457</v>
       </c>
       <c r="EC1" t="s">
-        <v>422</v>
+        <v>458</v>
       </c>
       <c r="ED1" t="s">
-        <v>423</v>
+        <v>459</v>
       </c>
       <c r="EE1" t="s">
-        <v>424</v>
+        <v>460</v>
       </c>
       <c r="EF1" t="s">
-        <v>425</v>
+        <v>461</v>
       </c>
       <c r="EG1" t="s">
-        <v>426</v>
+        <v>462</v>
       </c>
       <c r="EH1" t="s">
-        <v>427</v>
-      </c>
-      <c r="EI1" t="s">
-        <v>428</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="2" spans="3:140" x14ac:dyDescent="0.2">
-      <c r="U2" t="s">
-        <v>487</v>
-      </c>
-      <c r="V2" t="s">
-        <v>488</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>441</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>489</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>490</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>491</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>492</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>493</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>494</v>
-      </c>
-      <c r="BK2" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="BL2" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="BM2" s="7" t="s">
-        <v>497</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>498</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="3" spans="3:140" x14ac:dyDescent="0.2">
-      <c r="U3" t="s">
-        <v>500</v>
-      </c>
-      <c r="V3" t="s">
-        <v>501</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>502</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>503</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>447</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>504</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>505</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>506</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>492</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>493</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>494</v>
-      </c>
-      <c r="BK3" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="BL3" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="BM3" s="7" t="s">
-        <v>507</v>
-      </c>
-      <c r="DZ3" t="s">
-        <v>508</v>
-      </c>
-      <c r="EA3" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="4" spans="3:140" x14ac:dyDescent="0.2">
-      <c r="U4" t="s">
-        <v>510</v>
-      </c>
-      <c r="V4" t="s">
-        <v>511</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>512</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>513</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>450</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>514</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>515</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>516</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>492</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>493</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>494</v>
-      </c>
-      <c r="BK4" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="BL4" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="BM4" s="7" t="s">
-        <v>517</v>
-      </c>
-      <c r="DZ4" t="s">
-        <v>508</v>
-      </c>
-      <c r="EA4" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="5" spans="3:140" x14ac:dyDescent="0.2">
-      <c r="U5" t="s">
-        <v>518</v>
-      </c>
-      <c r="V5" t="s">
-        <v>519</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>453</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>520</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>521</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>522</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>492</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>493</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>494</v>
-      </c>
-      <c r="BK5" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="BL5" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="BM5" s="7" t="s">
-        <v>523</v>
-      </c>
-      <c r="DZ5" t="s">
-        <v>508</v>
-      </c>
-      <c r="EA5" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="6" spans="3:140" x14ac:dyDescent="0.2">
-      <c r="U6" t="s">
-        <v>518</v>
-      </c>
-      <c r="V6" t="s">
-        <v>524</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>456</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>525</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>526</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>527</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>492</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>493</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>494</v>
-      </c>
-      <c r="BK6" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="BL6" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="BM6" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="DZ6" t="s">
-        <v>498</v>
-      </c>
-      <c r="EA6" t="s">
-        <v>499</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -4264,243 +3477,53 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="C1:O6"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>465</v>
       </c>
       <c r="G1" t="s">
-        <v>430</v>
+        <v>466</v>
       </c>
       <c r="H1" t="s">
-        <v>431</v>
+        <v>467</v>
       </c>
       <c r="I1" t="s">
-        <v>432</v>
+        <v>468</v>
       </c>
       <c r="J1" t="s">
-        <v>433</v>
+        <v>469</v>
       </c>
       <c r="K1" t="s">
-        <v>434</v>
+        <v>470</v>
       </c>
       <c r="L1" t="s">
-        <v>435</v>
+        <v>471</v>
       </c>
       <c r="M1" t="s">
-        <v>436</v>
-      </c>
-      <c r="N1" t="s">
-        <v>437</v>
-      </c>
-      <c r="O1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C3" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>449</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C4" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>450</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C5" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C6" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>456</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>440</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding lost reverse complement for allele
</commit_message>
<xml_diff>
--- a/datasheets/allele.xlsx
+++ b/datasheets/allele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oriol/Desktop/beacon-ri-tools-v2/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769AD7C2-E7F1-5B41-8032-C5FEE3647BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E2CFFB-65F9-1A4D-B8F8-BE83301C25DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analyses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="482">
   <si>
     <t>aligner</t>
   </si>
@@ -1036,6 +1036,9 @@
     <t>variation|state|location|type</t>
   </si>
   <si>
+    <t>variation|state|reverse_complement</t>
+  </si>
+  <si>
     <t>variation|state|seq_expr|location|_id</t>
   </si>
   <si>
@@ -1096,6 +1099,9 @@
     <t>var00001</t>
   </si>
   <si>
+    <t>taxonomy:1214</t>
+  </si>
+  <si>
     <t>q22.4</t>
   </si>
   <si>
@@ -1111,6 +1117,27 @@
     <t>ChromosomeLocation</t>
   </si>
   <si>
+    <t>taxonomy:6609</t>
+  </si>
+  <si>
+    <t>DefiniteRange</t>
+  </si>
+  <si>
+    <t>SequenceInterval</t>
+  </si>
+  <si>
+    <t>VRS:0101</t>
+  </si>
+  <si>
+    <t>SequenceLocation</t>
+  </si>
+  <si>
+    <t>DerivedSequenceExpression</t>
+  </si>
+  <si>
+    <t>Allele</t>
+  </si>
+  <si>
     <t>diseases|ageOfOnset</t>
   </si>
   <si>
@@ -1445,24 +1472,6 @@
   </si>
   <si>
     <t>runDate</t>
-  </si>
-  <si>
-    <t>taxonomy:6609</t>
-  </si>
-  <si>
-    <t>SequenceInterval</t>
-  </si>
-  <si>
-    <t>VRS:0101</t>
-  </si>
-  <si>
-    <t>SequenceLocation</t>
-  </si>
-  <si>
-    <t>DerivedSequenceExpression</t>
-  </si>
-  <si>
-    <t>DefiniteRange</t>
   </si>
 </sst>
 </file>
@@ -2528,15 +2537,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:ER2"/>
+  <dimension ref="A1:ES2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DT1" workbookViewId="0">
-      <selection activeCell="DV1" sqref="DV1"/>
+    <sheetView tabSelected="1" topLeftCell="EA1" workbookViewId="0">
+      <selection activeCell="EC2" sqref="EC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:148" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -2981,40 +2990,46 @@
       <c r="ER1" t="s">
         <v>351</v>
       </c>
+      <c r="ES1" t="s">
+        <v>352</v>
+      </c>
     </row>
-    <row r="2" spans="1:148" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>357</v>
       </c>
       <c r="BZ2">
         <v>22</v>
       </c>
       <c r="CB2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="CH2" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="CN2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="CP2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="CQ2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="DJ2" t="s">
-        <v>473</v>
+        <v>363</v>
       </c>
       <c r="DU2">
         <v>1</v>
@@ -3023,19 +3038,25 @@
         <v>0</v>
       </c>
       <c r="DW2" t="s">
-        <v>478</v>
+        <v>364</v>
       </c>
       <c r="DY2" t="s">
-        <v>474</v>
+        <v>365</v>
       </c>
       <c r="DZ2" t="s">
-        <v>475</v>
+        <v>366</v>
       </c>
       <c r="EB2" t="s">
-        <v>476</v>
-      </c>
-      <c r="EP2" s="2" t="s">
-        <v>477</v>
+        <v>367</v>
+      </c>
+      <c r="EC2" t="b">
+        <v>1</v>
+      </c>
+      <c r="EQ2" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3055,91 +3076,91 @@
   <sheetData>
     <row r="1" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="B1" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="C1" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="D1" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="E1" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="F1" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="G1" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="H1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="I1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="J1" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="K1" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="L1" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="M1" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="N1" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="O1" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="P1" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="Q1" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="R1" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="S1" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="T1" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="U1" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="V1" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="W1" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="X1" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="Y1" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="Z1" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="AA1" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="AB1" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="AC1" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="AD1" t="s">
         <v>3</v>
@@ -3148,193 +3169,193 @@
         <v>5</v>
       </c>
       <c r="AF1" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="AG1" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="AH1" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="AI1" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="AJ1" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="AK1" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="AL1" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="AM1" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="AN1" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="AO1" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="AP1" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="AQ1" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="AR1" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="AS1" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="AT1" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="AU1" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="AV1" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="AW1" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="AX1" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="AY1" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="AZ1" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="BA1" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="BB1" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="BC1" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="BD1" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="BE1" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="BF1" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="BG1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="BH1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="BI1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="BJ1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="BK1" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="BL1" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="BM1" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="BN1" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="BO1" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="BP1" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
       <c r="BQ1" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="BR1" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="BS1" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="BT1" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="BU1" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="BV1" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="BW1" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="BX1" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="BY1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="BZ1" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="CA1" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="CB1" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="CC1" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="CD1" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="CE1" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="CF1" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="CG1" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="CH1" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="CI1" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="CJ1" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="CK1" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="CL1" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="CM1" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
       <c r="CN1" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="CO1" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="CP1" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="CQ1" t="s">
         <v>56</v>
@@ -3436,37 +3457,37 @@
         <v>88</v>
       </c>
       <c r="DX1" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="DY1" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="DZ1" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="EA1" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="EB1" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="EC1" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
       <c r="ED1" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="EE1" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="EF1" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="EG1" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="EH1" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -3499,31 +3520,31 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="F1" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="G1" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="H1" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="I1" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
       <c r="J1" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="K1" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
       <c r="L1" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="M1" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>